<commit_message>
Add a new version of the crawler to support multiple columns
</commit_message>
<xml_diff>
--- a/docs/_static/xlsx/tab_Tipo_tribunale.xlsx
+++ b/docs/_static/xlsx/tab_Tipo_tribunale.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t xml:space="preserve">   </t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Tribunale Estero</t>
+  </si>
+  <si>
+    <t>Avvocato/Notaio</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -514,18 +517,38 @@
         <v>5</v>
       </c>
       <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="D6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -560,4 +583,172 @@
   <pageSetup paperSize="0" firstPageNumber="4294967295" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all/>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46268D90-0CBF-4B8F-9DFC-FE62FBBB51E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2757A45-81BD-44C4-B924-BFB78F8928BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D436EF22-8427-4DEC-8809-372359FBDEFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>